<commit_message>
V1 of SAM gold mappings
</commit_message>
<xml_diff>
--- a/docs/data-maps/cts-silver-attr-map.xlsx
+++ b/docs/data-maps/cts-silver-attr-map.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\defra\ls-keeper-data-api\docs\data-maps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{130F0F4E-AD1A-4A36-996B-039356E7834E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{322A1E79-897B-4475-913E-51580FE764C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1900" yWindow="1900" windowWidth="25540" windowHeight="14320" activeTab="3" xr2:uid="{1BA62C16-295B-4239-B5A9-F8E1565DE45D}"/>
+    <workbookView xWindow="3760" yWindow="3760" windowWidth="23810" windowHeight="16020" activeTab="3" xr2:uid="{1BA62C16-295B-4239-B5A9-F8E1565DE45D}"/>
   </bookViews>
   <sheets>
     <sheet name="CTS CPHHolding" sheetId="1" r:id="rId1"/>
@@ -73,7 +73,7 @@
     <author>MarkGent1</author>
   </authors>
   <commentList>
-    <comment ref="A3" authorId="0" shapeId="0" xr:uid="{8984CC06-0820-467A-9586-FAEBA63D2A43}">
+    <comment ref="A12" authorId="0" shapeId="0" xr:uid="{7FB15A68-CB7E-4E68-800B-C34D5382D65A}">
       <text>
         <r>
           <rPr>
@@ -93,8 +93,8 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-1 = SAM
-2 = CTS</t>
+SAM
+CTS</t>
         </r>
       </text>
     </comment>
@@ -103,7 +103,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="119">
   <si>
     <t>BATCH_ID</t>
   </si>
@@ -399,9 +399,6 @@
     <t>Required Y|N</t>
   </si>
   <si>
-    <t>Assume this is for Source System Id (e.g. CTS or SAM)?</t>
-  </si>
-  <si>
     <t>Roles[].EffectiveFromData</t>
   </si>
   <si>
@@ -451,6 +448,18 @@
   </si>
   <si>
     <t>RoleTypeName</t>
+  </si>
+  <si>
+    <t>Enum or string value</t>
+  </si>
+  <si>
+    <t>Not sure what this is?</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>LOV Lookup? Not sure what this is?</t>
   </si>
 </sst>
 </file>
@@ -944,7 +953,7 @@
   <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="37.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1233,7 +1242,7 @@
   <dimension ref="A1:F31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="37.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1371,12 +1380,10 @@
         <v>53</v>
       </c>
       <c r="C10" s="21" t="s">
-        <v>98</v>
+        <v>118</v>
       </c>
       <c r="E10" s="10"/>
-      <c r="F10" s="10" t="s">
-        <v>95</v>
-      </c>
+      <c r="F10" s="10"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" s="7" t="s">
@@ -1591,7 +1598,7 @@
         <v>50</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D25" s="7"/>
       <c r="E25" s="6" t="s">
@@ -1606,7 +1613,7 @@
         <v>51</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C26" s="7"/>
       <c r="D26" s="7"/>
@@ -1619,7 +1626,7 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B27" s="7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C27" s="7" t="s">
         <v>64</v>
@@ -1632,7 +1639,7 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B28" s="9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C28" s="9" t="s">
         <v>65</v>
@@ -1646,10 +1653,10 @@
     <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29" s="7"/>
       <c r="B29" s="7" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C29" s="9" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D29" s="7"/>
       <c r="E29" s="8"/>
@@ -1686,7 +1693,7 @@
   <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="37.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1829,12 +1836,10 @@
         <v>53</v>
       </c>
       <c r="C10" s="21" t="s">
-        <v>98</v>
+        <v>118</v>
       </c>
       <c r="E10" s="10"/>
-      <c r="F10" s="10" t="s">
-        <v>95</v>
-      </c>
+      <c r="F10" s="10"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" s="7" t="s">
@@ -2043,7 +2048,7 @@
         <v>50</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D25" s="7"/>
       <c r="E25" s="6" t="s">
@@ -2058,7 +2063,7 @@
         <v>51</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C26" s="7"/>
       <c r="D26" s="7"/>
@@ -2071,7 +2076,7 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B27" s="7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C27" s="7" t="s">
         <v>73</v>
@@ -2084,7 +2089,7 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B28" s="7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C28" s="9" t="s">
         <v>65</v>
@@ -2098,10 +2103,10 @@
     <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29" s="7"/>
       <c r="B29" s="7" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C29" s="9" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D29" s="7"/>
       <c r="E29" s="7"/>
@@ -2127,10 +2132,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D4D2152-A6DC-4F95-8C3A-8E01B67DF0E8}">
-  <dimension ref="A1:F32"/>
+  <dimension ref="A1:F33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="37.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2262,102 +2267,103 @@
         <v>53</v>
       </c>
       <c r="C9" s="21" t="s">
-        <v>98</v>
+        <v>118</v>
       </c>
       <c r="E9" s="10"/>
-      <c r="F9" s="10" t="s">
+      <c r="F9" s="10"/>
+    </row>
+    <row r="10" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B10" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="C10" s="21"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="10" t="s">
         <v>95</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A10" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="D10" s="7"/>
-      <c r="E10" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="F10" s="6" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="C11" s="7"/>
+        <v>76</v>
+      </c>
       <c r="D11" s="7"/>
       <c r="E11" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A12" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="F11" s="6" t="s">
+      <c r="F12" s="6" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B12" s="7" t="s">
-        <v>102</v>
-      </c>
-      <c r="C12" s="7" t="s">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B13" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="C13" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="D12" s="7"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="8" t="s">
+      <c r="D13" s="7"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B13" s="9" t="s">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B14" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="C13" s="9" t="s">
+      <c r="C14" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="D13" s="7"/>
-      <c r="E13" s="10"/>
-      <c r="F13" s="10" t="s">
+      <c r="D14" s="7"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="10" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A14" s="9"/>
-      <c r="B14" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="C14" s="9" t="s">
-        <v>113</v>
-      </c>
-      <c r="D14" s="9"/>
-      <c r="E14" s="10"/>
-      <c r="F14" s="8" t="s">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A15" s="9"/>
+      <c r="B15" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="D15" s="9"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="8" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="F15" s="7"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="F16" s="7"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B17" s="7"/>
-      <c r="C17" s="7"/>
-      <c r="D17" s="7"/>
-      <c r="E17" s="8"/>
       <c r="F17" s="7"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A18" s="7"/>
+      <c r="B18" s="7"/>
       <c r="C18" s="7"/>
       <c r="D18" s="7"/>
-      <c r="E18" s="6"/>
+      <c r="E18" s="8"/>
       <c r="F18" s="7"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.35">
@@ -2371,26 +2377,27 @@
       <c r="A20" s="7"/>
       <c r="C20" s="7"/>
       <c r="D20" s="7"/>
-      <c r="E20"/>
+      <c r="E20" s="6"/>
       <c r="F20" s="7"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21" s="7"/>
-      <c r="B21" s="7"/>
       <c r="C21" s="7"/>
       <c r="D21" s="7"/>
-      <c r="E21" s="8"/>
+      <c r="E21"/>
       <c r="F21" s="7"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" s="7"/>
+      <c r="B22" s="7"/>
       <c r="C22" s="7"/>
       <c r="D22" s="7"/>
-      <c r="E22" s="6"/>
+      <c r="E22" s="8"/>
       <c r="F22" s="7"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23" s="7"/>
+      <c r="C23" s="7"/>
       <c r="D23" s="7"/>
       <c r="E23" s="6"/>
       <c r="F23" s="7"/>
@@ -2415,7 +2422,6 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27" s="7"/>
-      <c r="B27" s="7"/>
       <c r="D27" s="7"/>
       <c r="E27" s="6"/>
       <c r="F27" s="7"/>
@@ -2423,31 +2429,30 @@
     <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28" s="7"/>
       <c r="B28" s="7"/>
-      <c r="C28" s="7"/>
       <c r="D28" s="7"/>
       <c r="E28" s="6"/>
       <c r="F28" s="7"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A29" s="7"/>
       <c r="B29" s="7"/>
       <c r="C29" s="7"/>
       <c r="D29" s="7"/>
-      <c r="E29" s="8"/>
+      <c r="E29" s="6"/>
       <c r="F29" s="7"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B30" s="7"/>
-      <c r="C30" s="9"/>
+      <c r="C30" s="7"/>
       <c r="D30" s="7"/>
-      <c r="E30" s="10"/>
+      <c r="E30" s="8"/>
       <c r="F30" s="7"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A31" s="7"/>
       <c r="B31" s="7"/>
-      <c r="C31" s="7"/>
+      <c r="C31" s="9"/>
       <c r="D31" s="7"/>
-      <c r="E31" s="7"/>
+      <c r="E31" s="10"/>
       <c r="F31" s="7"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.35">
@@ -2457,6 +2462,14 @@
       <c r="D32" s="7"/>
       <c r="E32" s="7"/>
       <c r="F32" s="7"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A33" s="7"/>
+      <c r="B33" s="7"/>
+      <c r="C33" s="7"/>
+      <c r="D33" s="7"/>
+      <c r="E33" s="7"/>
+      <c r="F33" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2468,10 +2481,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92185A0C-3B74-494C-B406-F6014CF815ED}">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="44.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2492,73 +2505,84 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3" s="7" t="s">
-        <v>53</v>
+      <c r="A3" t="s">
+        <v>110</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>104</v>
-      </c>
-      <c r="C3" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="B4" s="19" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>105</v>
+      <c r="A5" s="20" t="s">
+        <v>108</v>
       </c>
       <c r="B5" s="19" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A6" s="20" t="s">
-        <v>109</v>
+      <c r="A6" s="7" t="s">
+        <v>106</v>
       </c>
       <c r="B6" s="19" t="s">
-        <v>104</v>
+        <v>103</v>
+      </c>
+      <c r="C6" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="7" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B7" s="19" t="s">
-        <v>104</v>
-      </c>
-      <c r="C7" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="7" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="B8" s="19" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="7" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B9" s="19" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A10" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="B10" s="19" t="s">
-        <v>104</v>
+        <v>103</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A11" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B11" s="19" t="s">
+        <v>117</v>
+      </c>
+      <c r="C11" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A12" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="B12" s="19" t="s">
+        <v>103</v>
+      </c>
+      <c r="C12" t="s">
+        <v>115</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Minor tweaks to mapping attributes
</commit_message>
<xml_diff>
--- a/docs/data-maps/cts-silver-attr-map.xlsx
+++ b/docs/data-maps/cts-silver-attr-map.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\defra\ls-keeper-data-api\docs\data-maps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{322A1E79-897B-4475-913E-51580FE764C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC0CAA36-B0FA-4C69-9B18-62D24EFBED21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3760" yWindow="3760" windowWidth="23810" windowHeight="16020" activeTab="3" xr2:uid="{1BA62C16-295B-4239-B5A9-F8E1565DE45D}"/>
+    <workbookView xWindow="14960" yWindow="110" windowWidth="23580" windowHeight="11220" activeTab="1" xr2:uid="{1BA62C16-295B-4239-B5A9-F8E1565DE45D}"/>
   </bookViews>
   <sheets>
     <sheet name="CTS CPHHolding" sheetId="1" r:id="rId1"/>
@@ -73,6 +73,31 @@
     <author>MarkGent1</author>
   </authors>
   <commentList>
+    <comment ref="A11" authorId="0" shapeId="0" xr:uid="{87D1E56C-1C24-4BA8-BAC6-DE60B2C62A8F}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>MarkGent1:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Person
+Company</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="A12" authorId="0" shapeId="0" xr:uid="{7FB15A68-CB7E-4E68-800B-C34D5382D65A}">
       <text>
         <r>
@@ -103,7 +128,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="118">
   <si>
     <t>BATCH_ID</t>
   </si>
@@ -453,30 +478,20 @@
     <t>Enum or string value</t>
   </si>
   <si>
-    <t>Not sure what this is?</t>
-  </si>
-  <si>
-    <t>?</t>
-  </si>
-  <si>
-    <t>LOV Lookup? Not sure what this is?</t>
+    <t>Person or Business (rules tbc)</t>
+  </si>
+  <si>
+    <t>Person</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -529,6 +544,19 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -577,12 +605,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -591,10 +619,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -603,39 +634,33 @@
     <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -953,7 +978,7 @@
   <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="37.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -983,22 +1008,22 @@
       <c r="F1" s="2"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="16" t="s">
         <v>87</v>
       </c>
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="16" t="s">
         <v>90</v>
       </c>
-      <c r="C2" s="18"/>
-      <c r="E2" s="18" t="s">
+      <c r="C2" s="17"/>
+      <c r="E2" s="17" t="s">
         <v>88</v>
       </c>
-      <c r="F2" s="18" t="s">
+      <c r="F2" s="17" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="E3" s="6"/>
+      <c r="E3" s="5"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B4" s="4" t="s">
@@ -1007,8 +1032,8 @@
       <c r="C4" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8" t="s">
+      <c r="E4" s="7"/>
+      <c r="F4" s="7" t="s">
         <v>68</v>
       </c>
     </row>
@@ -1016,8 +1041,8 @@
       <c r="B5" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8" t="s">
+      <c r="E5" s="7"/>
+      <c r="F5" s="7" t="s">
         <v>83</v>
       </c>
     </row>
@@ -1028,21 +1053,21 @@
       <c r="B6" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="E6" s="6">
+      <c r="E6" s="5">
         <v>1</v>
       </c>
-      <c r="F6" s="6">
+      <c r="F6" s="5">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="E7" s="6" t="s">
+      <c r="E7" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="F7" s="6" t="s">
+      <c r="F7" s="5" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1053,24 +1078,24 @@
       <c r="B8" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="E8" s="6" t="s">
+      <c r="E8" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="F8" s="6" t="s">
+      <c r="F8" s="5" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A9" s="16" t="s">
+      <c r="A9" s="15" t="s">
         <v>85</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E9" s="6" t="s">
+      <c r="E9" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="F9" s="6" t="s">
+      <c r="F9" s="5" t="s">
         <v>32</v>
       </c>
     </row>
@@ -1081,10 +1106,10 @@
       <c r="B10" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="E10" s="6" t="s">
+      <c r="E10" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="F10" s="6" t="s">
+      <c r="F10" s="5" t="s">
         <v>42</v>
       </c>
     </row>
@@ -1095,10 +1120,10 @@
       <c r="B11" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E11" s="6" t="s">
+      <c r="E11" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="F11" s="6" t="s">
+      <c r="F11" s="5" t="s">
         <v>91</v>
       </c>
     </row>
@@ -1109,10 +1134,10 @@
       <c r="B12" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="E12" s="6" t="s">
+      <c r="E12" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="F12" s="6" t="s">
+      <c r="F12" s="5" t="s">
         <v>39</v>
       </c>
     </row>
@@ -1123,10 +1148,10 @@
       <c r="B13" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="E13" s="6" t="s">
+      <c r="E13" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="F13" s="6" t="s">
+      <c r="F13" s="5" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1137,10 +1162,10 @@
       <c r="B14" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="E14" s="6" t="s">
+      <c r="E14" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="F14" s="6" t="s">
+      <c r="F14" s="5" t="s">
         <v>37</v>
       </c>
     </row>
@@ -1165,10 +1190,10 @@
       <c r="B16" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="E16" s="6" t="s">
+      <c r="E16" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="F16" s="6" t="s">
+      <c r="F16" s="5" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1179,10 +1204,10 @@
       <c r="B17" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="E17" s="6" t="s">
+      <c r="E17" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="F17" s="6" t="s">
+      <c r="F17" s="5" t="s">
         <v>34</v>
       </c>
     </row>
@@ -1193,10 +1218,10 @@
       <c r="B18" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="E18" s="6" t="s">
+      <c r="E18" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="F18" s="6" t="s">
+      <c r="F18" s="5" t="s">
         <v>35</v>
       </c>
     </row>
@@ -1207,10 +1232,10 @@
       <c r="B19" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="E19" s="6" t="s">
+      <c r="E19" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="F19" s="6" t="s">
+      <c r="F19" s="5" t="s">
         <v>41</v>
       </c>
     </row>
@@ -1221,10 +1246,10 @@
       <c r="B20" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="E20" s="6" t="s">
+      <c r="E20" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="F20" s="6" t="s">
+      <c r="F20" s="5" t="s">
         <v>40</v>
       </c>
     </row>
@@ -1241,8 +1266,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3100E8FE-84E0-4402-ABEF-EAA4A47A0DB9}">
   <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="37.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1251,7 +1276,7 @@
     <col min="2" max="2" width="36.36328125" style="4" customWidth="1"/>
     <col min="3" max="3" width="47.7265625" style="4" customWidth="1"/>
     <col min="4" max="4" width="5.81640625" style="4" customWidth="1"/>
-    <col min="5" max="5" width="32.453125" style="6" customWidth="1"/>
+    <col min="5" max="5" width="32.453125" style="5" customWidth="1"/>
     <col min="6" max="16384" width="37.54296875" style="4"/>
   </cols>
   <sheetData>
@@ -1265,50 +1290,50 @@
       <c r="C1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="10" t="s">
         <v>29</v>
       </c>
       <c r="F1" s="2"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="16" t="s">
         <v>92</v>
       </c>
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="16" t="s">
         <v>93</v>
       </c>
-      <c r="C2" s="18"/>
-      <c r="E2" s="18" t="s">
+      <c r="C2" s="17"/>
+      <c r="E2" s="17" t="s">
         <v>88</v>
       </c>
-      <c r="F2" s="18" t="s">
+      <c r="F2" s="17" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3" s="7"/>
-      <c r="F3" s="7"/>
+      <c r="A3" s="6"/>
+      <c r="F3" s="6"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4" s="7"/>
+      <c r="A4" s="6"/>
       <c r="B4" s="4" t="s">
         <v>80</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8" t="s">
+      <c r="E4" s="7"/>
+      <c r="F4" s="7" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A5" s="7"/>
+      <c r="A5" s="6"/>
       <c r="B5" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8" t="s">
+      <c r="E5" s="7"/>
+      <c r="F5" s="7" t="s">
         <v>83</v>
       </c>
     </row>
@@ -1319,161 +1344,163 @@
       <c r="B6" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="8" t="s">
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="F6" s="8" t="s">
+      <c r="F6" s="7" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="8" t="s">
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="F7" s="8" t="s">
+      <c r="F7" s="7" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A8" s="15" t="s">
+      <c r="A8" s="14" t="s">
         <v>86</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="8" t="s">
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="F8" s="8" t="s">
+      <c r="F8" s="7" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A9" s="15" t="s">
+      <c r="A9" s="14" t="s">
         <v>85</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C9" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="D9" s="7"/>
-      <c r="E9" s="6" t="s">
+      <c r="D9" s="6"/>
+      <c r="E9" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="F9" s="6" t="s">
+      <c r="F9" s="5" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="9" t="s">
+    <row r="10" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B10" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="C10" s="21" t="s">
-        <v>118</v>
-      </c>
-      <c r="E10" s="10"/>
-      <c r="F10" s="10"/>
+      <c r="C10" s="20" t="s">
+        <v>116</v>
+      </c>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9" t="s">
+        <v>117</v>
+      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A11" s="7" t="s">
+      <c r="A11" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="C11" s="7"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="8" t="s">
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="F11" s="8" t="s">
+      <c r="F11" s="7" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A12" s="7" t="s">
+      <c r="A12" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="B12" s="7" t="s">
+      <c r="B12" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="C12" s="7"/>
-      <c r="D12" s="7"/>
-      <c r="E12" s="8" t="s">
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="F12" s="8" t="s">
+      <c r="F12" s="7" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A13" s="7" t="s">
+      <c r="A13" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="B13" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="8" t="s">
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="F13" s="8" t="s">
+      <c r="F13" s="7" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A14" s="7" t="s">
+      <c r="A14" s="6" t="s">
         <v>46</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C14" s="7"/>
-      <c r="D14" s="7"/>
-      <c r="E14" s="6" t="s">
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="F14" s="6" t="s">
+      <c r="F14" s="5" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A15" s="7" t="s">
+      <c r="A15" s="6" t="s">
         <v>47</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C15" s="7"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="6" t="s">
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="F15" s="6" t="s">
+      <c r="F15" s="5" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A16" s="7" t="s">
+      <c r="A16" s="6" t="s">
         <v>48</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="C16" s="7"/>
-      <c r="D16" s="7"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
       <c r="E16" t="s">
         <v>72</v>
       </c>
@@ -1482,203 +1509,203 @@
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A17" s="12" t="s">
+      <c r="A17" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="B17" s="12"/>
-      <c r="C17" s="12" t="s">
+      <c r="B17" s="11"/>
+      <c r="C17" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="D17" s="7"/>
+      <c r="D17" s="6"/>
       <c r="E17"/>
       <c r="F17"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A18" s="12" t="s">
+      <c r="A18" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="B18" s="12"/>
-      <c r="C18" s="12" t="s">
+      <c r="B18" s="11"/>
+      <c r="C18" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="D18" s="7"/>
+      <c r="D18" s="6"/>
       <c r="E18"/>
       <c r="F18"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A19" s="12" t="s">
+      <c r="A19" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="B19" s="12"/>
-      <c r="C19" s="12" t="s">
+      <c r="B19" s="11"/>
+      <c r="C19" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="D19" s="7"/>
-      <c r="E19" s="8"/>
-      <c r="F19" s="8"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="7"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A20" s="7" t="s">
+      <c r="A20" s="6" t="s">
         <v>4</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="C20" s="7"/>
-      <c r="D20" s="7"/>
-      <c r="E20" s="6" t="s">
+      <c r="C20" s="6"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="F20" s="6" t="s">
+      <c r="F20" s="5" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A21" s="7" t="s">
+      <c r="A21" s="6" t="s">
         <v>7</v>
       </c>
       <c r="B21" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="D21" s="7"/>
-      <c r="E21" s="6" t="s">
+      <c r="D21" s="6"/>
+      <c r="E21" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="F21" s="6" t="s">
+      <c r="F21" s="5" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A22" s="7" t="s">
+      <c r="A22" s="6" t="s">
         <v>6</v>
       </c>
       <c r="B22" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="D22" s="7"/>
-      <c r="E22" s="6" t="s">
+      <c r="D22" s="6"/>
+      <c r="E22" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="F22" s="6" t="s">
+      <c r="F22" s="5" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A23" s="7" t="s">
+      <c r="A23" s="6" t="s">
         <v>5</v>
       </c>
       <c r="B23" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="D23" s="7"/>
-      <c r="E23" s="6" t="s">
+      <c r="D23" s="6"/>
+      <c r="E23" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="F23" s="6" t="s">
+      <c r="F23" s="5" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A24" s="7" t="s">
+      <c r="A24" s="6" t="s">
         <v>8</v>
       </c>
       <c r="B24" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="D24" s="7"/>
-      <c r="E24" s="6" t="s">
+      <c r="D24" s="6"/>
+      <c r="E24" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="F24" s="6" t="s">
+      <c r="F24" s="5" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A25" s="7" t="s">
+      <c r="A25" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="B25" s="7" t="s">
+      <c r="B25" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="D25" s="7"/>
-      <c r="E25" s="6" t="s">
+      <c r="D25" s="6"/>
+      <c r="E25" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="F25" s="6" t="s">
+      <c r="F25" s="5" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A26" s="7" t="s">
+      <c r="A26" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="B26" s="7" t="s">
+      <c r="B26" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="C26" s="7"/>
-      <c r="D26" s="7"/>
-      <c r="E26" s="6" t="s">
+      <c r="C26" s="6"/>
+      <c r="D26" s="6"/>
+      <c r="E26" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="F26" s="6" t="s">
+      <c r="F26" s="5" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B27" s="7" t="s">
+      <c r="B27" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="C27" s="7" t="s">
+      <c r="C27" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="D27" s="7"/>
-      <c r="E27" s="8"/>
-      <c r="F27" s="8" t="s">
+      <c r="D27" s="6"/>
+      <c r="E27" s="7"/>
+      <c r="F27" s="7" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B28" s="9" t="s">
+      <c r="B28" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="C28" s="9" t="s">
+      <c r="C28" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="D28" s="7"/>
-      <c r="E28" s="10"/>
-      <c r="F28" s="10" t="s">
+      <c r="D28" s="6"/>
+      <c r="E28" s="9"/>
+      <c r="F28" s="9" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A29" s="7"/>
-      <c r="B29" s="7" t="s">
+      <c r="A29" s="6"/>
+      <c r="B29" s="6" t="s">
         <v>113</v>
       </c>
-      <c r="C29" s="9" t="s">
+      <c r="C29" s="8" t="s">
         <v>112</v>
       </c>
-      <c r="D29" s="7"/>
-      <c r="E29" s="8"/>
-      <c r="F29" s="7" t="s">
+      <c r="D29" s="6"/>
+      <c r="E29" s="7"/>
+      <c r="F29" s="6" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A30" s="7"/>
-      <c r="B30" s="7"/>
-      <c r="C30" s="7"/>
-      <c r="D30" s="7"/>
-      <c r="E30" s="8"/>
-      <c r="F30" s="7"/>
+      <c r="A30" s="6"/>
+      <c r="B30" s="6"/>
+      <c r="C30" s="6"/>
+      <c r="D30" s="6"/>
+      <c r="E30" s="7"/>
+      <c r="F30" s="6"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A31" s="7"/>
-      <c r="B31" s="7"/>
-      <c r="C31" s="7"/>
-      <c r="D31" s="7"/>
-      <c r="E31" s="8"/>
-      <c r="F31" s="7"/>
+      <c r="A31" s="6"/>
+      <c r="B31" s="6"/>
+      <c r="C31" s="6"/>
+      <c r="D31" s="6"/>
+      <c r="E31" s="7"/>
+      <c r="F31" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1693,7 +1720,7 @@
   <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C38" sqref="C38"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="37.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1723,48 +1750,48 @@
       <c r="F1" s="2"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="16" t="s">
         <v>92</v>
       </c>
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="16" t="s">
         <v>93</v>
       </c>
-      <c r="C2" s="18"/>
-      <c r="E2" s="18" t="s">
+      <c r="C2" s="17"/>
+      <c r="E2" s="17" t="s">
         <v>88</v>
       </c>
-      <c r="F2" s="18" t="s">
+      <c r="F2" s="17" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3" s="7"/>
-      <c r="B3" s="7"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="7"/>
+      <c r="A3" s="6"/>
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="6"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4" s="7"/>
+      <c r="A4" s="6"/>
       <c r="B4" s="4" t="s">
         <v>80</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8" t="s">
+      <c r="E4" s="7"/>
+      <c r="F4" s="7" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A5" s="7"/>
+      <c r="A5" s="6"/>
       <c r="B5" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8" t="s">
+      <c r="E5" s="7"/>
+      <c r="F5" s="7" t="s">
         <v>83</v>
       </c>
     </row>
@@ -1775,161 +1802,163 @@
       <c r="B6" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="8" t="s">
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="F6" s="8" t="s">
+      <c r="F6" s="7" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="8" t="s">
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="F7" s="8" t="s">
+      <c r="F7" s="7" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A8" s="15" t="s">
+      <c r="A8" s="14" t="s">
         <v>86</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="8" t="s">
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="F8" s="8" t="s">
+      <c r="F8" s="7" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A9" s="15" t="s">
+      <c r="A9" s="14" t="s">
         <v>85</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C9" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="D9" s="7"/>
-      <c r="E9" s="6" t="s">
+      <c r="D9" s="6"/>
+      <c r="E9" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="F9" s="6" t="s">
+      <c r="F9" s="5" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="9" t="s">
+    <row r="10" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B10" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="C10" s="21" t="s">
-        <v>118</v>
-      </c>
-      <c r="E10" s="10"/>
-      <c r="F10" s="10"/>
+      <c r="C10" s="20" t="s">
+        <v>116</v>
+      </c>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9" t="s">
+        <v>117</v>
+      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A11" s="7" t="s">
+      <c r="A11" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="C11" s="7"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="8" t="s">
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="F11" s="8" t="s">
+      <c r="F11" s="7" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A12" s="7" t="s">
+      <c r="A12" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="B12" s="7" t="s">
+      <c r="B12" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="C12" s="7"/>
-      <c r="D12" s="7"/>
-      <c r="E12" s="8" t="s">
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="F12" s="8" t="s">
+      <c r="F12" s="7" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A13" s="7" t="s">
+      <c r="A13" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="B13" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="8" t="s">
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="F13" s="8" t="s">
+      <c r="F13" s="7" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A14" s="7" t="s">
+      <c r="A14" s="6" t="s">
         <v>46</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C14" s="7"/>
-      <c r="D14" s="7"/>
-      <c r="E14" s="6" t="s">
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="F14" s="6" t="s">
+      <c r="F14" s="5" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A15" s="7" t="s">
+      <c r="A15" s="6" t="s">
         <v>47</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C15" s="7"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="6" t="s">
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="F15" s="6" t="s">
+      <c r="F15" s="5" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A16" s="7" t="s">
+      <c r="A16" s="6" t="s">
         <v>48</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="C16" s="7"/>
-      <c r="D16" s="7"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
       <c r="E16" t="s">
         <v>72</v>
       </c>
@@ -1937,190 +1966,190 @@
         <v>72</v>
       </c>
     </row>
-    <row r="17" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="12" t="s">
+    <row r="17" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="C17" s="12" t="s">
+      <c r="C17" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="E17" s="13"/>
-      <c r="F17" s="13"/>
-    </row>
-    <row r="18" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="12" t="s">
+      <c r="E17" s="12"/>
+      <c r="F17" s="12"/>
+    </row>
+    <row r="18" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="C18" s="12" t="s">
+      <c r="C18" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="E18" s="13"/>
-      <c r="F18" s="13"/>
-    </row>
-    <row r="19" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="12" t="s">
+      <c r="E18" s="12"/>
+      <c r="F18" s="12"/>
+    </row>
+    <row r="19" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="C19" s="12" t="s">
+      <c r="C19" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="E19" s="14"/>
-      <c r="F19" s="14"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="13"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A20" s="7" t="s">
+      <c r="A20" s="6" t="s">
         <v>4</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="C20" s="7"/>
-      <c r="D20" s="7"/>
-      <c r="E20" s="6" t="s">
+      <c r="C20" s="6"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="F20" s="6" t="s">
+      <c r="F20" s="5" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A21" s="7" t="s">
+      <c r="A21" s="6" t="s">
         <v>7</v>
       </c>
       <c r="B21" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="D21" s="7"/>
-      <c r="E21" s="6" t="s">
+      <c r="D21" s="6"/>
+      <c r="E21" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="F21" s="6" t="s">
+      <c r="F21" s="5" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A22" s="7" t="s">
+      <c r="A22" s="6" t="s">
         <v>6</v>
       </c>
       <c r="B22" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="D22" s="7"/>
-      <c r="E22" s="6" t="s">
+      <c r="D22" s="6"/>
+      <c r="E22" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="F22" s="6" t="s">
+      <c r="F22" s="5" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A23" s="7" t="s">
+      <c r="A23" s="6" t="s">
         <v>5</v>
       </c>
       <c r="B23" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="D23" s="7"/>
-      <c r="E23" s="6" t="s">
+      <c r="D23" s="6"/>
+      <c r="E23" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="F23" s="6" t="s">
+      <c r="F23" s="5" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A24" s="7" t="s">
+      <c r="A24" s="6" t="s">
         <v>8</v>
       </c>
       <c r="B24" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="D24" s="7"/>
-      <c r="E24" s="6" t="s">
+      <c r="D24" s="6"/>
+      <c r="E24" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="F24" s="6" t="s">
+      <c r="F24" s="5" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A25" s="7" t="s">
+      <c r="A25" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="B25" s="7" t="s">
+      <c r="B25" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="D25" s="7"/>
-      <c r="E25" s="6" t="s">
+      <c r="D25" s="6"/>
+      <c r="E25" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="F25" s="6" t="s">
+      <c r="F25" s="5" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A26" s="7" t="s">
+      <c r="A26" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="B26" s="7" t="s">
+      <c r="B26" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="C26" s="7"/>
-      <c r="D26" s="7"/>
-      <c r="E26" s="6" t="s">
+      <c r="C26" s="6"/>
+      <c r="D26" s="6"/>
+      <c r="E26" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="F26" s="6" t="s">
+      <c r="F26" s="5" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B27" s="7" t="s">
+      <c r="B27" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="C27" s="7" t="s">
+      <c r="C27" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="D27" s="7"/>
-      <c r="E27" s="8"/>
-      <c r="F27" s="8" t="s">
+      <c r="D27" s="6"/>
+      <c r="E27" s="7"/>
+      <c r="F27" s="7" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B28" s="7" t="s">
+      <c r="B28" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="C28" s="9" t="s">
+      <c r="C28" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="D28" s="7"/>
-      <c r="E28" s="10"/>
-      <c r="F28" s="10" t="s">
+      <c r="D28" s="6"/>
+      <c r="E28" s="9"/>
+      <c r="F28" s="9" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A29" s="7"/>
-      <c r="B29" s="7" t="s">
+      <c r="A29" s="6"/>
+      <c r="B29" s="6" t="s">
         <v>113</v>
       </c>
-      <c r="C29" s="9" t="s">
+      <c r="C29" s="8" t="s">
         <v>112</v>
       </c>
-      <c r="D29" s="7"/>
-      <c r="E29" s="7"/>
-      <c r="F29" s="8" t="s">
+      <c r="D29" s="6"/>
+      <c r="E29" s="6"/>
+      <c r="F29" s="7" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A30" s="7"/>
-      <c r="B30" s="7"/>
-      <c r="C30" s="7"/>
-      <c r="D30" s="7"/>
-      <c r="E30" s="7"/>
-      <c r="F30" s="7"/>
+      <c r="A30" s="6"/>
+      <c r="B30" s="6"/>
+      <c r="C30" s="6"/>
+      <c r="D30" s="6"/>
+      <c r="E30" s="6"/>
+      <c r="F30" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2134,8 +2163,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D4D2152-A6DC-4F95-8C3A-8E01B67DF0E8}">
   <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="37.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2165,39 +2194,39 @@
       <c r="F1" s="2"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="16" t="s">
         <v>92</v>
       </c>
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="16" t="s">
         <v>94</v>
       </c>
-      <c r="C2" s="18"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="18" t="s">
+      <c r="C2" s="17"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="17" t="s">
         <v>88</v>
       </c>
-      <c r="F2" s="18" t="s">
+      <c r="F2" s="17" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3" s="7"/>
-      <c r="B3" s="7"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="7"/>
+      <c r="A3" s="6"/>
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="6"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4" s="7"/>
+      <c r="A4" s="6"/>
       <c r="B4" s="4" t="s">
         <v>80</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8" t="s">
+      <c r="E4" s="7"/>
+      <c r="F4" s="7" t="s">
         <v>68</v>
       </c>
     </row>
@@ -2208,268 +2237,270 @@
       <c r="B5" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="7"/>
-      <c r="D5" s="7"/>
-      <c r="E5" s="8" t="s">
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="F5" s="8" t="s">
+      <c r="F5" s="7" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="8" t="s">
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="F6" s="8" t="s">
+      <c r="F6" s="7" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" s="15" t="s">
+      <c r="A7" s="14" t="s">
         <v>85</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="6" t="s">
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="F7" s="6" t="s">
+      <c r="F7" s="5" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A8" s="15" t="s">
+      <c r="A8" s="14" t="s">
         <v>86</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="8" t="s">
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="F8" s="8" t="s">
+      <c r="F8" s="7" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="9" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="9" t="s">
+    <row r="9" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B9" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="C9" s="21" t="s">
-        <v>118</v>
-      </c>
-      <c r="E9" s="10"/>
-      <c r="F9" s="10"/>
-    </row>
-    <row r="10" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="9" t="s">
+      <c r="C9" s="20" t="s">
+        <v>116</v>
+      </c>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B10" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="C10" s="21"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="10" t="s">
+      <c r="C10" s="20"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A11" s="7" t="s">
+      <c r="A11" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="D11" s="7"/>
-      <c r="E11" s="6" t="s">
+      <c r="D11" s="6"/>
+      <c r="E11" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="F11" s="6" t="s">
+      <c r="F11" s="5" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A12" s="7" t="s">
+      <c r="A12" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="B12" s="7" t="s">
+      <c r="B12" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="C12" s="7"/>
-      <c r="D12" s="7"/>
-      <c r="E12" s="6" t="s">
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="F12" s="6" t="s">
+      <c r="F12" s="5" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B13" s="7" t="s">
+      <c r="B13" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="C13" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="D13" s="7"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="8" t="s">
+      <c r="D13" s="6"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B14" s="9" t="s">
+      <c r="B14" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="C14" s="9" t="s">
+      <c r="C14" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="D14" s="7"/>
-      <c r="E14" s="10"/>
-      <c r="F14" s="10" t="s">
+      <c r="D14" s="6"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="9" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A15" s="9"/>
-      <c r="B15" s="7" t="s">
+      <c r="A15" s="8"/>
+      <c r="B15" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="C15" s="9" t="s">
+      <c r="C15" s="8" t="s">
         <v>112</v>
       </c>
-      <c r="D15" s="9"/>
-      <c r="E15" s="10"/>
-      <c r="F15" s="8" t="s">
+      <c r="D15" s="8"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="7" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="F16" s="7"/>
+      <c r="F16" s="6"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="F17" s="7"/>
+      <c r="F17" s="6"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B18" s="7"/>
-      <c r="C18" s="7"/>
-      <c r="D18" s="7"/>
-      <c r="E18" s="8"/>
-      <c r="F18" s="7"/>
+      <c r="B18" s="6"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="6"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A19" s="7"/>
-      <c r="C19" s="7"/>
-      <c r="D19" s="7"/>
-      <c r="E19" s="6"/>
-      <c r="F19" s="7"/>
+      <c r="A19" s="6"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="6"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A20" s="7"/>
-      <c r="C20" s="7"/>
-      <c r="D20" s="7"/>
-      <c r="E20" s="6"/>
-      <c r="F20" s="7"/>
+      <c r="A20" s="6"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="6"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A21" s="7"/>
-      <c r="C21" s="7"/>
-      <c r="D21" s="7"/>
+      <c r="A21" s="6"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
       <c r="E21"/>
-      <c r="F21" s="7"/>
+      <c r="F21" s="6"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A22" s="7"/>
-      <c r="B22" s="7"/>
-      <c r="C22" s="7"/>
-      <c r="D22" s="7"/>
-      <c r="E22" s="8"/>
-      <c r="F22" s="7"/>
+      <c r="A22" s="6"/>
+      <c r="B22" s="6"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="7"/>
+      <c r="F22" s="6"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A23" s="7"/>
-      <c r="C23" s="7"/>
-      <c r="D23" s="7"/>
-      <c r="E23" s="6"/>
-      <c r="F23" s="7"/>
+      <c r="A23" s="6"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="6"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A24" s="7"/>
-      <c r="D24" s="7"/>
-      <c r="E24" s="6"/>
-      <c r="F24" s="7"/>
+      <c r="A24" s="6"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="6"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A25" s="7"/>
-      <c r="D25" s="7"/>
-      <c r="E25" s="6"/>
-      <c r="F25" s="7"/>
+      <c r="A25" s="6"/>
+      <c r="D25" s="6"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="6"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A26" s="7"/>
-      <c r="D26" s="7"/>
-      <c r="E26" s="6"/>
-      <c r="F26" s="7"/>
+      <c r="A26" s="6"/>
+      <c r="D26" s="6"/>
+      <c r="E26" s="5"/>
+      <c r="F26" s="6"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A27" s="7"/>
-      <c r="D27" s="7"/>
-      <c r="E27" s="6"/>
-      <c r="F27" s="7"/>
+      <c r="A27" s="6"/>
+      <c r="D27" s="6"/>
+      <c r="E27" s="5"/>
+      <c r="F27" s="6"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A28" s="7"/>
-      <c r="B28" s="7"/>
-      <c r="D28" s="7"/>
-      <c r="E28" s="6"/>
-      <c r="F28" s="7"/>
+      <c r="A28" s="6"/>
+      <c r="B28" s="6"/>
+      <c r="D28" s="6"/>
+      <c r="E28" s="5"/>
+      <c r="F28" s="6"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A29" s="7"/>
-      <c r="B29" s="7"/>
-      <c r="C29" s="7"/>
-      <c r="D29" s="7"/>
-      <c r="E29" s="6"/>
-      <c r="F29" s="7"/>
+      <c r="A29" s="6"/>
+      <c r="B29" s="6"/>
+      <c r="C29" s="6"/>
+      <c r="D29" s="6"/>
+      <c r="E29" s="5"/>
+      <c r="F29" s="6"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B30" s="7"/>
-      <c r="C30" s="7"/>
-      <c r="D30" s="7"/>
-      <c r="E30" s="8"/>
-      <c r="F30" s="7"/>
+      <c r="B30" s="6"/>
+      <c r="C30" s="6"/>
+      <c r="D30" s="6"/>
+      <c r="E30" s="7"/>
+      <c r="F30" s="6"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B31" s="7"/>
-      <c r="C31" s="9"/>
-      <c r="D31" s="7"/>
-      <c r="E31" s="10"/>
-      <c r="F31" s="7"/>
+      <c r="B31" s="6"/>
+      <c r="C31" s="8"/>
+      <c r="D31" s="6"/>
+      <c r="E31" s="9"/>
+      <c r="F31" s="6"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A32" s="7"/>
-      <c r="B32" s="7"/>
-      <c r="C32" s="7"/>
-      <c r="D32" s="7"/>
-      <c r="E32" s="7"/>
-      <c r="F32" s="7"/>
+      <c r="A32" s="6"/>
+      <c r="B32" s="6"/>
+      <c r="C32" s="6"/>
+      <c r="D32" s="6"/>
+      <c r="E32" s="6"/>
+      <c r="F32" s="6"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A33" s="7"/>
-      <c r="B33" s="7"/>
-      <c r="C33" s="7"/>
-      <c r="D33" s="7"/>
-      <c r="E33" s="7"/>
-      <c r="F33" s="7"/>
+      <c r="A33" s="6"/>
+      <c r="B33" s="6"/>
+      <c r="C33" s="6"/>
+      <c r="D33" s="6"/>
+      <c r="E33" s="6"/>
+      <c r="F33" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2484,7 +2515,7 @@
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="44.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2508,7 +2539,7 @@
       <c r="A3" t="s">
         <v>110</v>
       </c>
-      <c r="B3" s="19" t="s">
+      <c r="B3" s="18" t="s">
         <v>103</v>
       </c>
     </row>
@@ -2516,23 +2547,23 @@
       <c r="A4" t="s">
         <v>104</v>
       </c>
-      <c r="B4" s="19" t="s">
+      <c r="B4" s="18" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A5" s="20" t="s">
+      <c r="A5" s="19" t="s">
         <v>108</v>
       </c>
-      <c r="B5" s="19" t="s">
+      <c r="B5" s="18" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="B6" s="19" t="s">
+      <c r="B6" s="18" t="s">
         <v>103</v>
       </c>
       <c r="C6" t="s">
@@ -2540,45 +2571,45 @@
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="B7" s="19" t="s">
+      <c r="B7" s="18" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="B8" s="19" t="s">
+      <c r="B8" s="18" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A9" s="7" t="s">
+      <c r="A9" s="6" t="s">
         <v>111</v>
       </c>
-      <c r="B9" s="19" t="s">
+      <c r="B9" s="18" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A11" s="7" t="s">
+      <c r="A11" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="B11" s="19" t="s">
-        <v>117</v>
+      <c r="B11" s="18" t="s">
+        <v>103</v>
       </c>
       <c r="C11" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A12" s="7" t="s">
+      <c r="A12" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="B12" s="19" t="s">
+      <c r="B12" s="18" t="s">
         <v>103</v>
       </c>
       <c r="C12" t="s">

</xml_diff>

<commit_message>
Added SAM Herd mapping steps and tests.
</commit_message>
<xml_diff>
--- a/docs/data-maps/cts-silver-attr-map.xlsx
+++ b/docs/data-maps/cts-silver-attr-map.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\defra\ls-keeper-data-api\docs\data-maps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC0CAA36-B0FA-4C69-9B18-62D24EFBED21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EBC4823-B43D-4BF0-BC23-258776A0328A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14960" yWindow="110" windowWidth="23580" windowHeight="11220" activeTab="1" xr2:uid="{1BA62C16-295B-4239-B5A9-F8E1565DE45D}"/>
+    <workbookView xWindow="20" yWindow="11440" windowWidth="17840" windowHeight="9460" activeTab="2" xr2:uid="{1BA62C16-295B-4239-B5A9-F8E1565DE45D}"/>
   </bookViews>
   <sheets>
     <sheet name="CTS CPHHolding" sheetId="1" r:id="rId1"/>
@@ -978,7 +978,7 @@
   <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="37.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1266,8 +1266,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3100E8FE-84E0-4402-ABEF-EAA4A47A0DB9}">
   <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="37.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1719,8 +1719,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E2870F0-993A-4B7C-96BC-DBEBA6330BDA}">
   <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="37.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2163,8 +2163,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D4D2152-A6DC-4F95-8C3A-8E01B67DF0E8}">
   <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="37.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Complete implementation of the Insert Sam Holding Silver mappings step (#30)
* Getting all the SAM silver step and mappings inline with CTS + empty tests.

* Added seed type services and Sam Holding mapper + tests.

* SAM Holding and Party mappings added.

* Added SAM Herd mapping steps and tests.

* Fixed linting issues

---------

Co-authored-by: Mark Gent <Mark.Gent@homesengland.gov.uk>
</commit_message>
<xml_diff>
--- a/docs/data-maps/cts-silver-attr-map.xlsx
+++ b/docs/data-maps/cts-silver-attr-map.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\defra\ls-keeper-data-api\docs\data-maps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC0CAA36-B0FA-4C69-9B18-62D24EFBED21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EBC4823-B43D-4BF0-BC23-258776A0328A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14960" yWindow="110" windowWidth="23580" windowHeight="11220" activeTab="1" xr2:uid="{1BA62C16-295B-4239-B5A9-F8E1565DE45D}"/>
+    <workbookView xWindow="20" yWindow="11440" windowWidth="17840" windowHeight="9460" activeTab="2" xr2:uid="{1BA62C16-295B-4239-B5A9-F8E1565DE45D}"/>
   </bookViews>
   <sheets>
     <sheet name="CTS CPHHolding" sheetId="1" r:id="rId1"/>
@@ -978,7 +978,7 @@
   <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="37.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1266,8 +1266,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3100E8FE-84E0-4402-ABEF-EAA4A47A0DB9}">
   <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="37.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1719,8 +1719,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E2870F0-993A-4B7C-96BC-DBEBA6330BDA}">
   <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="37.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2163,8 +2163,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D4D2152-A6DC-4F95-8C3A-8E01B67DF0E8}">
   <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="37.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Updated CTS Mappings and Tests.
</commit_message>
<xml_diff>
--- a/docs/data-maps/cts-silver-attr-map.xlsx
+++ b/docs/data-maps/cts-silver-attr-map.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://defra-my.sharepoint.com/personal/mark_gent_defra_gov_uk/Documents/Documents/KRDS/Mappings/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\defra\ls-keeper-data-api\docs\data-maps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="43" documentId="13_ncr:1_{4EBC4823-B43D-4BF0-BC23-258776A0328A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A3824C88-3482-4C13-BBCB-D53918E1198B}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{866EA191-100D-4255-8CAA-4166B9FFF950}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29085" yWindow="1140" windowWidth="28515" windowHeight="9510" activeTab="3" xr2:uid="{1BA62C16-295B-4239-B5A9-F8E1565DE45D}"/>
+    <workbookView xWindow="-40" yWindow="5600" windowWidth="24250" windowHeight="15280" xr2:uid="{1BA62C16-295B-4239-B5A9-F8E1565DE45D}"/>
   </bookViews>
   <sheets>
     <sheet name="CTS CPHHolding" sheetId="1" r:id="rId1"/>
@@ -128,7 +128,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="122">
   <si>
     <t>BATCH_ID</t>
   </si>
@@ -493,17 +493,14 @@
     <t>Livestock Keeper</t>
   </si>
   <si>
-    <t>Roles[].RoleTypeCode</t>
-  </si>
-  <si>
-    <t>RoleTypeCode</t>
+    <t>SiteIdentifierType</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -559,13 +556,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -614,7 +604,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -670,12 +660,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -698,9 +682,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -738,7 +722,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -844,7 +828,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -986,7 +970,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -996,8 +980,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C5EF1DC-D2AC-4A4B-82BB-D60D1A15ED0A}">
   <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="37.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1289,10 +1273,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3100E8FE-84E0-4402-ABEF-EAA4A47A0DB9}">
-  <dimension ref="A1:F31"/>
+  <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="37.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1702,39 +1686,27 @@
         <v>64</v>
       </c>
     </row>
-    <row r="29" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B29" s="21" t="s">
-        <v>121</v>
-      </c>
-      <c r="C29" s="21" t="s">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A29" s="6"/>
+      <c r="B29" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="C29" s="8" t="s">
         <v>105</v>
       </c>
-      <c r="E29" s="22"/>
-      <c r="F29" s="22" t="s">
-        <v>115</v>
+      <c r="D29" s="6"/>
+      <c r="E29" s="7"/>
+      <c r="F29" s="6" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A30" s="6"/>
-      <c r="B30" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="C30" s="8" t="s">
-        <v>105</v>
-      </c>
+      <c r="B30" s="6"/>
+      <c r="C30" s="6"/>
       <c r="D30" s="6"/>
       <c r="E30" s="7"/>
-      <c r="F30" s="6" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A31" s="6"/>
-      <c r="B31" s="6"/>
-      <c r="C31" s="6"/>
-      <c r="D31" s="6"/>
-      <c r="E31" s="7"/>
-      <c r="F31" s="6"/>
+      <c r="F30" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1746,10 +1718,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E2870F0-993A-4B7C-96BC-DBEBA6330BDA}">
-  <dimension ref="A1:F30"/>
+  <dimension ref="A1:F29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="37.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2158,28 +2130,17 @@
         <v>64</v>
       </c>
     </row>
-    <row r="29" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B29" s="21" t="s">
-        <v>121</v>
-      </c>
-      <c r="C29" s="21" t="s">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A29" s="6"/>
+      <c r="B29" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="C29" s="8" t="s">
         <v>105</v>
       </c>
-      <c r="F29" s="22" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A30" s="6"/>
-      <c r="B30" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="C30" s="8" t="s">
-        <v>105</v>
-      </c>
-      <c r="D30" s="6"/>
-      <c r="E30" s="6"/>
-      <c r="F30" s="7" t="s">
+      <c r="D29" s="6"/>
+      <c r="E29" s="6"/>
+      <c r="F29" s="7" t="s">
         <v>120</v>
       </c>
     </row>
@@ -2193,10 +2154,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D4D2152-A6DC-4F95-8C3A-8E01B67DF0E8}">
-  <dimension ref="A1:F33"/>
+  <dimension ref="A1:F32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A15" sqref="A15:XFD15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="37.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2403,37 +2364,31 @@
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A15" s="8"/>
       <c r="B15" s="6" t="s">
-        <v>122</v>
+        <v>107</v>
       </c>
       <c r="C15" s="8" t="s">
         <v>105</v>
       </c>
-      <c r="D15" s="8"/>
       <c r="F15" s="7" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B16" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="C16" s="8" t="s">
-        <v>105</v>
-      </c>
-      <c r="F16" s="7" t="s">
-        <v>120</v>
-      </c>
+      <c r="F16" s="6"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B17" s="6"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="7"/>
       <c r="F17" s="6"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B18" s="6"/>
+      <c r="A18" s="6"/>
       <c r="C18" s="6"/>
       <c r="D18" s="6"/>
-      <c r="E18" s="7"/>
+      <c r="E18" s="5"/>
       <c r="F18" s="6"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.35">
@@ -2447,27 +2402,26 @@
       <c r="A20" s="6"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
-      <c r="E20" s="5"/>
+      <c r="E20"/>
       <c r="F20" s="6"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21" s="6"/>
+      <c r="B21" s="6"/>
       <c r="C21" s="6"/>
       <c r="D21" s="6"/>
-      <c r="E21"/>
+      <c r="E21" s="7"/>
       <c r="F21" s="6"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" s="6"/>
-      <c r="B22" s="6"/>
       <c r="C22" s="6"/>
       <c r="D22" s="6"/>
-      <c r="E22" s="7"/>
+      <c r="E22" s="5"/>
       <c r="F22" s="6"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23" s="6"/>
-      <c r="C23" s="6"/>
       <c r="D23" s="6"/>
       <c r="E23" s="5"/>
       <c r="F23" s="6"/>
@@ -2492,6 +2446,7 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27" s="6"/>
+      <c r="B27" s="6"/>
       <c r="D27" s="6"/>
       <c r="E27" s="5"/>
       <c r="F27" s="6"/>
@@ -2499,30 +2454,31 @@
     <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28" s="6"/>
       <c r="B28" s="6"/>
+      <c r="C28" s="6"/>
       <c r="D28" s="6"/>
       <c r="E28" s="5"/>
       <c r="F28" s="6"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A29" s="6"/>
       <c r="B29" s="6"/>
       <c r="C29" s="6"/>
       <c r="D29" s="6"/>
-      <c r="E29" s="5"/>
+      <c r="E29" s="7"/>
       <c r="F29" s="6"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B30" s="6"/>
-      <c r="C30" s="6"/>
+      <c r="C30" s="8"/>
       <c r="D30" s="6"/>
-      <c r="E30" s="7"/>
+      <c r="E30" s="9"/>
       <c r="F30" s="6"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A31" s="6"/>
       <c r="B31" s="6"/>
-      <c r="C31" s="8"/>
+      <c r="C31" s="6"/>
       <c r="D31" s="6"/>
-      <c r="E31" s="9"/>
+      <c r="E31" s="6"/>
       <c r="F31" s="6"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.35">
@@ -2532,14 +2488,6 @@
       <c r="D32" s="6"/>
       <c r="E32" s="6"/>
       <c r="F32" s="6"/>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A33" s="6"/>
-      <c r="B33" s="6"/>
-      <c r="C33" s="6"/>
-      <c r="D33" s="6"/>
-      <c r="E33" s="6"/>
-      <c r="F33" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2554,7 +2502,7 @@
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="44.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2633,6 +2581,14 @@
         <v>96</v>
       </c>
     </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A10" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="B10" s="18" t="s">
+        <v>96</v>
+      </c>
+    </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" s="6" t="s">
         <v>51</v>

</xml_diff>

<commit_message>
Update CTS & SAM bronze-silver mappings in solution and aggregate when multiple records occur (#43)
* Create branch in GH

* Updated silver mappings

* Renamed silverPartyRoleRelationships

* Updated CTS Mappings and Tests.

* Removed CPH from Sam Party

* Added PAON and SAON Descriptions

* Sam Holding and Herd silver maps updated.

* SAM holder and party mappings updated.

* Storing multiple silver sam holdings

* Updated SAM Silver Persistence steps using composite keys.

* Rejigging SAM Holder execution

* Moved the SAM mappings folder

* Sam Holder persistence step completed

* Moved Mappings folders and tests

* Added Sam Holder step tests

* Added Bronze data envelope and converters.

* CTS and SAM Silver steps completed

* Liniting changes.

---------

Co-authored-by: Mark Gent <Mark.Gent@homesengland.gov.uk>
</commit_message>
<xml_diff>
--- a/docs/data-maps/cts-silver-attr-map.xlsx
+++ b/docs/data-maps/cts-silver-attr-map.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\defra\ls-keeper-data-api\docs\data-maps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EBC4823-B43D-4BF0-BC23-258776A0328A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{866EA191-100D-4255-8CAA-4166B9FFF950}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="11440" windowWidth="17840" windowHeight="9460" activeTab="2" xr2:uid="{1BA62C16-295B-4239-B5A9-F8E1565DE45D}"/>
+    <workbookView xWindow="-40" yWindow="5600" windowWidth="24250" windowHeight="15280" xr2:uid="{1BA62C16-295B-4239-B5A9-F8E1565DE45D}"/>
   </bookViews>
   <sheets>
     <sheet name="CTS CPHHolding" sheetId="1" r:id="rId1"/>
@@ -81,7 +81,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>MarkGent1:</t>
         </r>
@@ -90,7 +90,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Person
@@ -128,7 +128,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="122">
   <si>
     <t>BATCH_ID</t>
   </si>
@@ -226,18 +226,12 @@
     <t>AH</t>
   </si>
   <si>
-    <t>12/345/6789</t>
-  </si>
-  <si>
     <t>0191 123 4567</t>
   </si>
   <si>
     <t>07795801234</t>
   </si>
   <si>
-    <t>NY 99568 79087</t>
-  </si>
-  <si>
     <t>Market Square</t>
   </si>
   <si>
@@ -322,18 +316,12 @@
     <t>Agent</t>
   </si>
   <si>
-    <t>Inferred as 'Agent'</t>
-  </si>
-  <si>
     <t>LOV Lookup / Internal Id</t>
   </si>
   <si>
     <t>1</t>
   </si>
   <si>
-    <t>C1000001</t>
-  </si>
-  <si>
     <t>10000000-0000-0000-0000-000000000001</t>
   </si>
   <si>
@@ -349,15 +337,6 @@
     <t>john.doe@email.co.uk</t>
   </si>
   <si>
-    <t>Inferred as 'Primary Keeper'</t>
-  </si>
-  <si>
-    <t>Primary Keeper</t>
-  </si>
-  <si>
-    <t>C1000002</t>
-  </si>
-  <si>
     <t>EffectiveFromData</t>
   </si>
   <si>
@@ -478,17 +457,50 @@
     <t>Enum or string value</t>
   </si>
   <si>
-    <t>Person or Business (rules tbc)</t>
-  </si>
-  <si>
     <t>Person</t>
+  </si>
+  <si>
+    <t>AG-3000123, AH-48/015/9000</t>
+  </si>
+  <si>
+    <t>3000123, 48/015/9000</t>
+  </si>
+  <si>
+    <t>Seem the wrong way around</t>
+  </si>
+  <si>
+    <t>NS 334567</t>
+  </si>
+  <si>
+    <t>Inferred as code 'AGENT'</t>
+  </si>
+  <si>
+    <t>AGENT</t>
+  </si>
+  <si>
+    <t>Person or Business (rules tbc) based on title?</t>
+  </si>
+  <si>
+    <t>25799721</t>
+  </si>
+  <si>
+    <t>Inferred as code 'LIVESTOCKKEEPER'</t>
+  </si>
+  <si>
+    <t>LIVESTOCKKEEPER</t>
+  </si>
+  <si>
+    <t>Livestock Keeper</t>
+  </si>
+  <si>
+    <t>SiteIdentifierType</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -543,19 +555,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -676,6 +675,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -977,8 +980,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C5EF1DC-D2AC-4A4B-82BB-D60D1A15ED0A}">
   <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="37.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -993,10 +996,10 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>28</v>
@@ -1009,17 +1012,17 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="16" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="C2" s="17"/>
       <c r="E2" s="17" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="F2" s="17" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
@@ -1027,23 +1030,23 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B4" s="4" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="E4" s="7"/>
       <c r="F4" s="7" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B5" s="4" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="E5" s="7"/>
       <c r="F5" s="7" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
@@ -1087,16 +1090,16 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" s="15" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>15</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>32</v>
+        <v>110</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>32</v>
+        <v>111</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
@@ -1107,10 +1110,10 @@
         <v>21</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
@@ -1121,10 +1124,10 @@
         <v>20</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
@@ -1134,11 +1137,14 @@
       <c r="B12" s="4" t="s">
         <v>22</v>
       </c>
+      <c r="C12" s="4" t="s">
+        <v>112</v>
+      </c>
       <c r="E12" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
@@ -1148,11 +1154,14 @@
       <c r="B13" s="4" t="s">
         <v>23</v>
       </c>
+      <c r="C13" s="4" t="s">
+        <v>112</v>
+      </c>
       <c r="E13" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.35">
@@ -1163,10 +1172,10 @@
         <v>24</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.35">
@@ -1177,10 +1186,10 @@
         <v>25</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.35">
@@ -1191,10 +1200,10 @@
         <v>26</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.35">
@@ -1205,10 +1214,10 @@
         <v>27</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.35">
@@ -1219,10 +1228,10 @@
         <v>19</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>35</v>
+        <v>113</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>35</v>
+        <v>113</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.35">
@@ -1233,10 +1242,10 @@
         <v>17</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.35">
@@ -1247,10 +1256,10 @@
         <v>18</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -1264,10 +1273,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3100E8FE-84E0-4402-ABEF-EAA4A47A0DB9}">
-  <dimension ref="A1:F31"/>
+  <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="37.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1282,10 +1291,10 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>28</v>
@@ -1297,17 +1306,17 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="16" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="C2" s="17"/>
       <c r="E2" s="17" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="F2" s="17" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
@@ -1317,24 +1326,24 @@
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="6"/>
       <c r="B4" s="4" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="E4" s="7"/>
       <c r="F4" s="7" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="6"/>
       <c r="B5" s="4" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="E5" s="7"/>
       <c r="F5" s="7" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
@@ -1347,10 +1356,10 @@
       <c r="C6" s="6"/>
       <c r="D6" s="6"/>
       <c r="E6" s="7" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
@@ -1368,101 +1377,101 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="14" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C8" s="6"/>
       <c r="D8" s="6"/>
       <c r="E8" s="7" t="s">
-        <v>67</v>
+        <v>117</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>67</v>
+        <v>117</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" s="14" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="B9" s="6" t="s">
         <v>15</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D9" s="6"/>
       <c r="E9" s="5" t="s">
-        <v>32</v>
+        <v>110</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>32</v>
+        <v>111</v>
       </c>
     </row>
     <row r="10" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B10" s="8" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C10" s="20" t="s">
         <v>116</v>
       </c>
       <c r="E10" s="9"/>
       <c r="F10" s="9" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" s="6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C11" s="6"/>
       <c r="D11" s="6"/>
       <c r="E11" s="7" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" s="6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C12" s="6"/>
       <c r="D12" s="6"/>
       <c r="E12" s="7" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" s="6" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C13" s="6"/>
       <c r="D13" s="6"/>
       <c r="E13" s="7" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" s="6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>26</v>
@@ -1470,15 +1479,15 @@
       <c r="C14" s="6"/>
       <c r="D14" s="6"/>
       <c r="E14" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" s="6" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>27</v>
@@ -1486,26 +1495,26 @@
       <c r="C15" s="6"/>
       <c r="D15" s="6"/>
       <c r="E15" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" s="6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C16" s="6"/>
       <c r="D16" s="6"/>
       <c r="E16" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="F16" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.35">
@@ -1514,7 +1523,7 @@
       </c>
       <c r="B17" s="11"/>
       <c r="C17" s="11" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="D17" s="6"/>
       <c r="E17"/>
@@ -1526,7 +1535,7 @@
       </c>
       <c r="B18" s="11"/>
       <c r="C18" s="11" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="D18" s="6"/>
       <c r="E18"/>
@@ -1538,7 +1547,7 @@
       </c>
       <c r="B19" s="11"/>
       <c r="C19" s="11" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="D19" s="6"/>
       <c r="E19" s="7"/>
@@ -1549,15 +1558,15 @@
         <v>4</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="5" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.35">
@@ -1565,14 +1574,14 @@
         <v>7</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D21" s="6"/>
       <c r="E21" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.35">
@@ -1580,14 +1589,14 @@
         <v>6</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D22" s="6"/>
       <c r="E22" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.35">
@@ -1595,14 +1604,14 @@
         <v>5</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D23" s="6"/>
       <c r="E23" s="5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.35">
@@ -1610,85 +1619,85 @@
         <v>8</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D24" s="6"/>
       <c r="E24" s="5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25" s="6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="D25" s="6"/>
       <c r="E25" s="5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26" s="6" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="C26" s="6"/>
       <c r="D26" s="6"/>
       <c r="E26" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B27" s="6" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>64</v>
+        <v>114</v>
       </c>
       <c r="D27" s="6"/>
       <c r="E27" s="7"/>
       <c r="F27" s="7" t="s">
-        <v>63</v>
+        <v>115</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B28" s="8" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D28" s="6"/>
       <c r="E28" s="9"/>
       <c r="F28" s="9" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29" s="6"/>
       <c r="B29" s="6" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="D29" s="6"/>
       <c r="E29" s="7"/>
       <c r="F29" s="6" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.35">
@@ -1699,28 +1708,20 @@
       <c r="E30" s="7"/>
       <c r="F30" s="6"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A31" s="6"/>
-      <c r="B31" s="6"/>
-      <c r="C31" s="6"/>
-      <c r="D31" s="6"/>
-      <c r="E31" s="7"/>
-      <c r="F31" s="6"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="E6:F6 E15:F15" numberStoredAsText="1"/>
+    <ignoredError sqref="E6:F6 E15:F15 E8:F8" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E2870F0-993A-4B7C-96BC-DBEBA6330BDA}">
-  <dimension ref="A1:F30"/>
+  <dimension ref="A1:F29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="37.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1735,10 +1736,10 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>28</v>
@@ -1751,17 +1752,17 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="16" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="C2" s="17"/>
       <c r="E2" s="17" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="F2" s="17" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
@@ -1775,24 +1776,24 @@
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="6"/>
       <c r="B4" s="4" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="E4" s="7"/>
       <c r="F4" s="7" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="6"/>
       <c r="B5" s="4" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="E5" s="7"/>
       <c r="F5" s="7" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
@@ -1805,10 +1806,10 @@
       <c r="C6" s="6"/>
       <c r="D6" s="6"/>
       <c r="E6" s="7" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
@@ -1826,101 +1827,101 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="14" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C8" s="6"/>
       <c r="D8" s="6"/>
       <c r="E8" s="7" t="s">
-        <v>75</v>
+        <v>117</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>75</v>
+        <v>117</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" s="14" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="B9" s="6" t="s">
         <v>15</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D9" s="6"/>
       <c r="E9" s="5" t="s">
-        <v>32</v>
+        <v>110</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>32</v>
+        <v>111</v>
       </c>
     </row>
     <row r="10" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B10" s="8" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C10" s="20" t="s">
         <v>116</v>
       </c>
       <c r="E10" s="9"/>
       <c r="F10" s="9" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" s="6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C11" s="6"/>
       <c r="D11" s="6"/>
       <c r="E11" s="7" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" s="6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C12" s="6"/>
       <c r="D12" s="6"/>
       <c r="E12" s="7" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" s="6" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C13" s="6"/>
       <c r="D13" s="6"/>
       <c r="E13" s="7" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" s="6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>26</v>
@@ -1928,15 +1929,15 @@
       <c r="C14" s="6"/>
       <c r="D14" s="6"/>
       <c r="E14" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" s="6" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>27</v>
@@ -1944,26 +1945,26 @@
       <c r="C15" s="6"/>
       <c r="D15" s="6"/>
       <c r="E15" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" s="6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C16" s="6"/>
       <c r="D16" s="6"/>
       <c r="E16" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="F16" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="17" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.35">
@@ -1971,7 +1972,7 @@
         <v>10</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="E17" s="12"/>
       <c r="F17" s="12"/>
@@ -1981,7 +1982,7 @@
         <v>11</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="E18" s="12"/>
       <c r="F18" s="12"/>
@@ -1991,7 +1992,7 @@
         <v>3</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="E19" s="13"/>
       <c r="F19" s="13"/>
@@ -2001,15 +2002,15 @@
         <v>4</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="5" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.35">
@@ -2017,14 +2018,14 @@
         <v>7</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D21" s="6"/>
       <c r="E21" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.35">
@@ -2032,14 +2033,14 @@
         <v>6</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D22" s="6"/>
       <c r="E22" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.35">
@@ -2047,14 +2048,14 @@
         <v>5</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D23" s="6"/>
       <c r="E23" s="5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.35">
@@ -2062,109 +2063,101 @@
         <v>8</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D24" s="6"/>
       <c r="E24" s="5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25" s="6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="D25" s="6"/>
       <c r="E25" s="5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26" s="6" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="C26" s="6"/>
       <c r="D26" s="6"/>
       <c r="E26" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B27" s="6" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>73</v>
+        <v>118</v>
       </c>
       <c r="D27" s="6"/>
       <c r="E27" s="7"/>
       <c r="F27" s="7" t="s">
-        <v>74</v>
+        <v>119</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B28" s="6" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D28" s="6"/>
       <c r="E28" s="9"/>
       <c r="F28" s="9" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29" s="6"/>
       <c r="B29" s="6" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="D29" s="6"/>
       <c r="E29" s="6"/>
       <c r="F29" s="7" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A30" s="6"/>
-      <c r="B30" s="6"/>
-      <c r="C30" s="6"/>
-      <c r="D30" s="6"/>
-      <c r="E30" s="6"/>
-      <c r="F30" s="6"/>
+        <v>120</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="E15:F15 E6:F6" numberStoredAsText="1"/>
+    <ignoredError sqref="E15:F15 E6:F6 E8:F8" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D4D2152-A6DC-4F95-8C3A-8E01B67DF0E8}">
-  <dimension ref="A1:F33"/>
+  <dimension ref="A1:F32"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A15" sqref="A15:XFD15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="37.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2179,10 +2172,10 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>28</v>
@@ -2195,18 +2188,18 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="16" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="C2" s="17"/>
       <c r="D2" s="6"/>
       <c r="E2" s="17" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="F2" s="17" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
@@ -2220,14 +2213,14 @@
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="6"/>
       <c r="B4" s="4" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="E4" s="7"/>
       <c r="F4" s="7" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
@@ -2240,10 +2233,10 @@
       <c r="C5" s="6"/>
       <c r="D5" s="6"/>
       <c r="E5" s="7" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
@@ -2261,140 +2254,141 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="14" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>15</v>
       </c>
       <c r="C7" s="6"/>
       <c r="D7" s="6"/>
-      <c r="E7" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>32</v>
+      <c r="E7" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="14" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C8" s="6"/>
       <c r="D8" s="6"/>
-      <c r="E8" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="F8" s="7" t="s">
-        <v>75</v>
+      <c r="E8" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="9" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B9" s="8" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C9" s="20" t="s">
         <v>116</v>
       </c>
       <c r="E9" s="9"/>
       <c r="F9" s="9" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
     </row>
     <row r="10" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B10" s="8" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="C10" s="20"/>
       <c r="E10" s="9"/>
       <c r="F10" s="9" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" s="6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="D11" s="6"/>
       <c r="E11" s="5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" s="6" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="C12" s="6"/>
       <c r="D12" s="6"/>
       <c r="E12" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B13" s="6" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="D13" s="6"/>
       <c r="E13" s="7"/>
       <c r="F13" s="7" t="s">
-        <v>74</v>
+        <v>119</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B14" s="8" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D14" s="6"/>
       <c r="E14" s="9"/>
       <c r="F14" s="9" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A15" s="8"/>
       <c r="B15" s="6" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>112</v>
-      </c>
-      <c r="D15" s="8"/>
-      <c r="E15" s="9"/>
+        <v>105</v>
+      </c>
       <c r="F15" s="7" t="s">
-        <v>74</v>
+        <v>120</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="F16" s="6"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B17" s="6"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="7"/>
       <c r="F17" s="6"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B18" s="6"/>
+      <c r="A18" s="6"/>
       <c r="C18" s="6"/>
       <c r="D18" s="6"/>
-      <c r="E18" s="7"/>
+      <c r="E18" s="5"/>
       <c r="F18" s="6"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.35">
@@ -2408,27 +2402,26 @@
       <c r="A20" s="6"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
-      <c r="E20" s="5"/>
+      <c r="E20"/>
       <c r="F20" s="6"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21" s="6"/>
+      <c r="B21" s="6"/>
       <c r="C21" s="6"/>
       <c r="D21" s="6"/>
-      <c r="E21"/>
+      <c r="E21" s="7"/>
       <c r="F21" s="6"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" s="6"/>
-      <c r="B22" s="6"/>
       <c r="C22" s="6"/>
       <c r="D22" s="6"/>
-      <c r="E22" s="7"/>
+      <c r="E22" s="5"/>
       <c r="F22" s="6"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23" s="6"/>
-      <c r="C23" s="6"/>
       <c r="D23" s="6"/>
       <c r="E23" s="5"/>
       <c r="F23" s="6"/>
@@ -2453,6 +2446,7 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27" s="6"/>
+      <c r="B27" s="6"/>
       <c r="D27" s="6"/>
       <c r="E27" s="5"/>
       <c r="F27" s="6"/>
@@ -2460,30 +2454,31 @@
     <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28" s="6"/>
       <c r="B28" s="6"/>
+      <c r="C28" s="6"/>
       <c r="D28" s="6"/>
       <c r="E28" s="5"/>
       <c r="F28" s="6"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A29" s="6"/>
       <c r="B29" s="6"/>
       <c r="C29" s="6"/>
       <c r="D29" s="6"/>
-      <c r="E29" s="5"/>
+      <c r="E29" s="7"/>
       <c r="F29" s="6"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B30" s="6"/>
-      <c r="C30" s="6"/>
+      <c r="C30" s="8"/>
       <c r="D30" s="6"/>
-      <c r="E30" s="7"/>
+      <c r="E30" s="9"/>
       <c r="F30" s="6"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A31" s="6"/>
       <c r="B31" s="6"/>
-      <c r="C31" s="8"/>
+      <c r="C31" s="6"/>
       <c r="D31" s="6"/>
-      <c r="E31" s="9"/>
+      <c r="E31" s="6"/>
       <c r="F31" s="6"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.35">
@@ -2494,18 +2489,10 @@
       <c r="E32" s="6"/>
       <c r="F32" s="6"/>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A33" s="6"/>
-      <c r="B33" s="6"/>
-      <c r="C33" s="6"/>
-      <c r="D33" s="6"/>
-      <c r="E33" s="6"/>
-      <c r="F33" s="6"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="E5:F5" numberStoredAsText="1"/>
+    <ignoredError sqref="E5:F5 E7:F7" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -2515,7 +2502,7 @@
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="44.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2526,10 +2513,10 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>28</v>
@@ -2537,83 +2524,91 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="B3" s="18" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="19" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="B5" s="18" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="6" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="B6" s="18" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="C6" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="6" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="B7" s="18" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="6" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="B8" s="18" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="6" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="B9" s="18" t="s">
-        <v>103</v>
+        <v>96</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A10" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="B10" s="18" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" s="6" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B11" s="18" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="C11" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" s="6" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="B12" s="18" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="C12" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
     </row>
   </sheetData>

</xml_diff>